<commit_message>
Update Communication Plan_Levi‘s CMS System SI_(JP-TKY).xlsx
</commit_message>
<xml_diff>
--- a/2019/东京店/99 项目管理/Communication Plan_Levi‘s CMS System SI_(JP-TKY).xlsx
+++ b/2019/东京店/99 项目管理/Communication Plan_Levi‘s CMS System SI_(JP-TKY).xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AF0B01-6709-4CD1-A062-F5C48D64A1FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="-216" windowWidth="14808" windowHeight="7980" activeTab="2"/>
+    <workbookView xWindow="972" yWindow="-108" windowWidth="22176" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="沟通计划" sheetId="3" r:id="rId1"/>
@@ -172,10 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
-  <si>
-    <t>CMS相关负责</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="66">
   <si>
     <t>数拓</t>
   </si>
@@ -187,12 +185,6 @@
   </si>
   <si>
     <t>Sapling</t>
-  </si>
-  <si>
-    <t>中间沟通</t>
-  </si>
-  <si>
-    <t>客户沟通、LED供应</t>
   </si>
   <si>
     <t>总包</t>
@@ -307,30 +299,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>项目管理支持</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>项目管理执行</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>日本现场实施负责</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>项目管理负责</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LED及配件供应</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>拼接屏及配件供应</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>LED供应商</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -354,11 +322,115 @@
     <t>jason@desound.com.cn</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>邵寿康</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sshao@levi.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IT PM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tshen@levi.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tony</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>总部市场部</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>业务部门负责人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jack Wu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vera Wong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VWong@LEVI.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jwu1@levi.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Penny</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phuang2@levi.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Henny</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hchen1@levi.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工程部负责人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>采购部负责人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目管理支持</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目管理负责</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目管理执行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日本现场实施负责</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拼接屏及配件供应</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED及配件供应</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>总体方案协调</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CMS供应商</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数拓负责人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -717,7 +789,7 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 2" xfId="1"/>
+    <cellStyle name="常规 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="超链接" xfId="2" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -755,7 +827,13 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="3" name="组合 2"/>
+        <xdr:cNvPr id="3" name="组合 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
@@ -768,7 +846,13 @@
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="36" name="文本框 1"/>
+          <xdr:cNvPr id="36" name="文本框 1">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000024000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr txBox="1"/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -904,7 +988,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="37" name="圆角矩形 36"/>
+          <xdr:cNvPr id="37" name="圆角矩形 36">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000025000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1148,7 +1238,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="38" name="圆角矩形 37"/>
+          <xdr:cNvPr id="38" name="圆角矩形 37">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000026000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1402,7 +1498,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="39" name="矩形 38"/>
+          <xdr:cNvPr id="39" name="矩形 38">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000027000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1564,7 +1666,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="40" name="矩形 39"/>
+          <xdr:cNvPr id="40" name="矩形 39">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000028000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1726,7 +1834,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="41" name="矩形 40"/>
+          <xdr:cNvPr id="41" name="矩形 40">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000029000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1888,7 +2002,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="42" name="矩形 41"/>
+          <xdr:cNvPr id="42" name="矩形 41">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00002A000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -2050,7 +2170,13 @@
       </xdr:sp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="43" name="肘形连接符 42"/>
+          <xdr:cNvPr id="43" name="肘形连接符 42">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00002B000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr>
             <a:endCxn id="41" idx="0"/>
           </xdr:cNvCxnSpPr>
@@ -2086,7 +2212,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="44" name="肘形连接符 43"/>
+          <xdr:cNvPr id="44" name="肘形连接符 43">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00002C000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr>
             <a:endCxn id="40" idx="0"/>
           </xdr:cNvCxnSpPr>
@@ -2122,7 +2254,13 @@
       </xdr:cxnSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="45" name="圆角矩形 44"/>
+          <xdr:cNvPr id="45" name="圆角矩形 44">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00002D000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -2366,7 +2504,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="46" name="圆角矩形 45"/>
+          <xdr:cNvPr id="46" name="圆角矩形 45">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00002E000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -2520,7 +2664,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="47" name="圆角矩形 46"/>
+          <xdr:cNvPr id="47" name="圆角矩形 46">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00002F000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -2706,7 +2856,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="48" name="圆角矩形 47"/>
+          <xdr:cNvPr id="48" name="圆角矩形 47">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000030000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -2884,7 +3040,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="49" name="圆角矩形 48"/>
+          <xdr:cNvPr id="49" name="圆角矩形 48">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000031000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -3046,7 +3208,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="51" name="矩形 50"/>
+          <xdr:cNvPr id="51" name="矩形 50">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000033000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -3208,7 +3376,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="52" name="矩形 51"/>
+          <xdr:cNvPr id="52" name="矩形 51">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000034000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -3362,7 +3536,13 @@
       </xdr:sp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="53" name="直接连接符 52"/>
+          <xdr:cNvPr id="53" name="直接连接符 52">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000035000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr>
             <a:stCxn id="46" idx="2"/>
             <a:endCxn id="49" idx="0"/>
@@ -3399,7 +3579,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="54" name="肘形连接符 53"/>
+          <xdr:cNvPr id="54" name="肘形连接符 53">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000036000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr>
             <a:stCxn id="42" idx="0"/>
           </xdr:cNvCxnSpPr>
@@ -3435,7 +3621,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="55" name="肘形连接符 54"/>
+          <xdr:cNvPr id="55" name="肘形连接符 54">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000037000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr>
             <a:stCxn id="51" idx="0"/>
           </xdr:cNvCxnSpPr>
@@ -3471,7 +3663,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="56" name="直接连接符 55"/>
+          <xdr:cNvPr id="56" name="直接连接符 55">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000038000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -3505,7 +3703,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="57" name="直接连接符 56"/>
+          <xdr:cNvPr id="57" name="直接连接符 56">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000039000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr>
             <a:stCxn id="51" idx="2"/>
             <a:endCxn id="52" idx="0"/>
@@ -3542,7 +3746,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="58" name="直接连接符 57"/>
+          <xdr:cNvPr id="58" name="直接连接符 57">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00003A000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr>
             <a:endCxn id="51" idx="1"/>
           </xdr:cNvCxnSpPr>
@@ -3579,7 +3789,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="61" name="直接连接符 60"/>
+          <xdr:cNvPr id="61" name="直接连接符 60">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00003D000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -3613,7 +3829,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="62" name="肘形连接符 61"/>
+          <xdr:cNvPr id="62" name="肘形连接符 61">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00003E000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr>
             <a:endCxn id="50" idx="2"/>
           </xdr:cNvCxnSpPr>
@@ -3649,7 +3871,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="65" name="直接连接符 64"/>
+          <xdr:cNvPr id="65" name="直接连接符 64">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000041000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -3683,7 +3911,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="66" name="直接连接符 65"/>
+          <xdr:cNvPr id="66" name="直接连接符 65">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000042000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr>
             <a:stCxn id="49" idx="2"/>
             <a:endCxn id="63" idx="0"/>
@@ -3720,7 +3954,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="67" name="直接连接符 66"/>
+          <xdr:cNvPr id="67" name="直接连接符 66">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000043000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -3754,7 +3994,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="68" name="直接连接符 67"/>
+          <xdr:cNvPr id="68" name="直接连接符 67">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000044000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -3788,7 +4034,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="69" name="肘形连接符 68"/>
+          <xdr:cNvPr id="69" name="肘形连接符 68">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000045000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -3824,7 +4076,13 @@
       </xdr:cxnSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="63" name="圆角矩形 62"/>
+          <xdr:cNvPr id="63" name="圆角矩形 62">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00003F000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -4013,7 +4271,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="59" name="圆角矩形 58"/>
+          <xdr:cNvPr id="59" name="圆角矩形 58">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00003B000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -4183,7 +4447,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="50" name="圆角矩形 49"/>
+          <xdr:cNvPr id="50" name="圆角矩形 49">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000032000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -14298,7 +14568,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -14373,6 +14643,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -14408,6 +14695,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -14583,12 +14887,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -14603,181 +14907,268 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="22"/>
+      <c r="B2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>40</v>
+      </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="E2" s="21" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
-      <c r="C3" s="22"/>
+      <c r="C3" s="22" t="s">
+        <v>44</v>
+      </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="E3" s="21" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
-      <c r="D4" s="3">
-        <v>13061735228</v>
-      </c>
+      <c r="D4" s="3"/>
       <c r="E4" s="21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="24" t="s">
-        <v>4</v>
+      <c r="A5" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
-      <c r="D5" s="3">
-        <v>13621728006</v>
-      </c>
+      <c r="D5" s="3"/>
       <c r="E5" s="21" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="25"/>
+      <c r="A6" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="B6" s="3" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
-      <c r="D6" s="3">
-        <v>13621964074</v>
-      </c>
+      <c r="D6" s="3"/>
       <c r="E6" s="21" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="26"/>
+      <c r="A7" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="B7" s="3" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
-      <c r="D7" s="3">
-        <v>13636570504</v>
-      </c>
+      <c r="D7" s="3"/>
       <c r="E7" s="21" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3">
-        <v>17721408226</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>47</v>
-      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="20" t="s">
-        <v>1</v>
+      <c r="A9" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" s="3">
-        <v>13621795963</v>
+        <v>13061735228</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="23" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="C10" s="22"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="4" t="s">
-        <v>43</v>
+      <c r="A11" s="24" t="s">
+        <v>3</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="C11" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="3">
+        <v>13621728006</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="25"/>
+      <c r="B12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="3">
+        <v>13621964074</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="26"/>
+      <c r="B13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="3">
+        <v>13636570504</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3">
+        <v>17721408226</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="3">
+        <v>13621795963</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="22"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A11:A13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E8" r:id="rId1"/>
-    <hyperlink ref="E5" r:id="rId2"/>
-    <hyperlink ref="E6" r:id="rId3"/>
-    <hyperlink ref="E7" r:id="rId4"/>
-    <hyperlink ref="E9" r:id="rId5"/>
-    <hyperlink ref="E4" r:id="rId6"/>
+    <hyperlink ref="E14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E12" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E13" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E15" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E2" r:id="rId7" xr:uid="{944D9B49-F332-4B0C-B0AA-E978154B12F0}"/>
+    <hyperlink ref="E3" r:id="rId8" xr:uid="{4BAB359C-D7A5-4862-82C4-50C0500D1B98}"/>
+    <hyperlink ref="E4" r:id="rId9" xr:uid="{1DECDD98-FA21-4F96-838C-72DB984F61A5}"/>
+    <hyperlink ref="E5" r:id="rId10" xr:uid="{ABA31A2D-5092-4500-A58C-18A3D261C08F}"/>
+    <hyperlink ref="E6" r:id="rId11" xr:uid="{746BE5E8-5F8B-451B-ACE7-220992397035}"/>
+    <hyperlink ref="E7" r:id="rId12" xr:uid="{46FFA19C-CC90-4F1A-AFB0-6D551082A1FE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14796,70 +15187,70 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.6">
       <c r="A1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>20</v>
-      </c>
       <c r="D1" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C2" s="13">
         <v>43609</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1">
@@ -14876,10 +15267,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>

</xml_diff>